<commit_message>
Daten hinzugefügt und angefangen zu bereinigen
</commit_message>
<xml_diff>
--- a/3.Semester/Datenanalyse/62111-0100_de.xlsx
+++ b/3.Semester/Datenanalyse/62111-0100_de.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Simon\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Simon\Desktop\Studium\3.Semester\Datenanalyse\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9E0E3B5E-D973-4FD5-A9B0-9D3599744E58}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{121A4FFA-E0F4-477F-8131-484BDAA0881B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21390" tabRatio="206" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -17,7 +17,7 @@
   </sheets>
   <calcPr calcId="0"/>
   <pivotCaches>
-    <pivotCache cacheId="23" r:id="rId2"/>
+    <pivotCache cacheId="0" r:id="rId2"/>
   </pivotCaches>
 </workbook>
 </file>
@@ -154,8 +154,8 @@
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="3">
     <numFmt numFmtId="44" formatCode="_-* #,##0.00\ &quot;€&quot;_-;\-* #,##0.00\ &quot;€&quot;_-;_-* &quot;-&quot;??\ &quot;€&quot;_-;_-@_-"/>
-    <numFmt numFmtId="165" formatCode="#,##0.00\ &quot;€&quot;"/>
-    <numFmt numFmtId="166" formatCode="_-* #,##0.00\ [$€-407]_-;\-* #,##0.00\ [$€-407]_-;_-* &quot;-&quot;??\ [$€-407]_-;_-@_-"/>
+    <numFmt numFmtId="164" formatCode="#,##0.00\ &quot;€&quot;"/>
+    <numFmt numFmtId="165" formatCode="_-* #,##0.00\ [$€-407]_-;\-* #,##0.00\ [$€-407]_-;_-* &quot;-&quot;??\ [$€-407]_-;_-@_-"/>
   </numFmts>
   <fonts count="5" x14ac:knownFonts="1">
     <font>
@@ -248,7 +248,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="44" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="25">
+  <cellXfs count="23">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
@@ -260,10 +260,10 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="165" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="166" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="44" fontId="1" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
@@ -275,17 +275,16 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="44" fontId="1" fillId="0" borderId="2" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="44" fontId="1" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="166" fontId="1" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="165" fontId="1" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="166" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="165" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="165" fontId="1" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="165" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" pivotButton="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -293,7 +292,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" indent="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
@@ -638,7 +636,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{98DF45F0-5427-42AF-ABAF-8B69541F96C8}" name="PivotTable4" cacheId="23" dataOnRows="1" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Werte" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="1">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{98DF45F0-5427-42AF-ABAF-8B69541F96C8}" name="PivotTable4" cacheId="0" dataOnRows="1" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Werte" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="2">
   <location ref="M3:P30" firstHeaderRow="1" firstDataRow="2" firstDataCol="1" rowPageCount="1" colPageCount="1"/>
   <pivotFields count="11">
     <pivotField axis="axisPage" multipleItemSelectionAllowed="1" showAll="0">
@@ -785,7 +783,7 @@
     <dataField name="Mittelwert von Hochschul- oder Universitätsabschluss" fld="9" subtotal="average" baseField="2" baseItem="0"/>
     <dataField name="Mittelwert von Ohne Angabe des Abschlusses" fld="10" subtotal="average" baseField="2" baseItem="0"/>
   </dataFields>
-  <chartFormats count="2">
+  <chartFormats count="4">
     <chartFormat chart="0" format="0" series="1">
       <pivotArea type="data" outline="0" fieldPosition="0">
         <references count="2">
@@ -799,6 +797,30 @@
       </pivotArea>
     </chartFormat>
     <chartFormat chart="0" format="1" series="1">
+      <pivotArea type="data" outline="0" fieldPosition="0">
+        <references count="2">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="0"/>
+          </reference>
+          <reference field="1" count="1" selected="0">
+            <x v="1"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </chartFormat>
+    <chartFormat chart="1" format="0" series="1">
+      <pivotArea type="data" outline="0" fieldPosition="0">
+        <references count="2">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="0"/>
+          </reference>
+          <reference field="1" count="1" selected="0">
+            <x v="0"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </chartFormat>
+    <chartFormat chart="1" format="1" series="1">
       <pivotArea type="data" outline="0" fieldPosition="0">
         <references count="2">
           <reference field="4294967294" count="1" selected="0">
@@ -1146,7 +1168,7 @@
       <pane xSplit="3" ySplit="4" topLeftCell="J5" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="N34" sqref="N34"/>
+      <selection pane="bottomRight" activeCell="M32" sqref="M32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.7109375" defaultRowHeight="13.5" x14ac:dyDescent="0.25"/>
@@ -1189,13 +1211,13 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:37" ht="38.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="20" t="s">
+      <c r="A1" s="15" t="s">
         <v>19</v>
       </c>
-      <c r="B1" s="20" t="s">
+      <c r="B1" s="15" t="s">
         <v>20</v>
       </c>
-      <c r="C1" s="20" t="s">
+      <c r="C1" s="15" t="s">
         <v>21</v>
       </c>
       <c r="D1" s="9" t="s">
@@ -1222,7 +1244,7 @@
       <c r="K1" s="9" t="s">
         <v>7</v>
       </c>
-      <c r="M1" s="21" t="s">
+      <c r="M1" s="20" t="s">
         <v>19</v>
       </c>
       <c r="N1" t="s">
@@ -1297,7 +1319,7 @@
         <v>3340</v>
       </c>
       <c r="M3"/>
-      <c r="N3" s="21" t="s">
+      <c r="N3" s="20" t="s">
         <v>24</v>
       </c>
       <c r="O3"/>
@@ -1354,7 +1376,7 @@
       <c r="K4" s="18">
         <v>1616</v>
       </c>
-      <c r="M4" s="21" t="s">
+      <c r="M4" s="20" t="s">
         <v>22</v>
       </c>
       <c r="N4" t="s">
@@ -1420,12 +1442,12 @@
       <c r="K5" s="18">
         <v>2459</v>
       </c>
-      <c r="M5" s="22" t="s">
+      <c r="M5" s="21" t="s">
         <v>13</v>
       </c>
-      <c r="N5" s="24"/>
-      <c r="O5" s="24"/>
-      <c r="P5" s="24"/>
+      <c r="N5"/>
+      <c r="O5"/>
+      <c r="P5"/>
       <c r="Q5"/>
       <c r="R5"/>
       <c r="S5"/>
@@ -1478,16 +1500,16 @@
       <c r="K6" s="18">
         <v>2139</v>
       </c>
-      <c r="M6" s="23" t="s">
+      <c r="M6" s="22" t="s">
         <v>25</v>
       </c>
-      <c r="N6" s="24">
+      <c r="N6">
         <v>3135</v>
       </c>
-      <c r="O6" s="24">
+      <c r="O6">
         <v>2193</v>
       </c>
-      <c r="P6" s="24">
+      <c r="P6">
         <v>2664</v>
       </c>
       <c r="Q6"/>
@@ -1544,16 +1566,16 @@
       <c r="K7" s="18">
         <v>3467</v>
       </c>
-      <c r="M7" s="23" t="s">
+      <c r="M7" s="22" t="s">
         <v>27</v>
       </c>
-      <c r="N7" s="24">
+      <c r="N7">
         <v>2655</v>
       </c>
-      <c r="O7" s="24">
+      <c r="O7">
         <v>2173</v>
       </c>
-      <c r="P7" s="24">
+      <c r="P7">
         <v>2414</v>
       </c>
       <c r="Q7"/>
@@ -1608,16 +1630,16 @@
       <c r="K8" s="18">
         <v>1660</v>
       </c>
-      <c r="M8" s="23" t="s">
+      <c r="M8" s="22" t="s">
         <v>29</v>
       </c>
-      <c r="N8" s="24">
+      <c r="N8">
         <v>3499</v>
       </c>
-      <c r="O8" s="24">
+      <c r="O8">
         <v>2617</v>
       </c>
-      <c r="P8" s="24">
+      <c r="P8">
         <v>3058</v>
       </c>
       <c r="Q8"/>
@@ -1674,16 +1696,16 @@
       <c r="K9" s="18">
         <v>2481</v>
       </c>
-      <c r="M9" s="23" t="s">
+      <c r="M9" s="22" t="s">
         <v>31</v>
       </c>
-      <c r="N9" s="24">
+      <c r="N9">
         <v>3456</v>
       </c>
-      <c r="O9" s="24">
+      <c r="O9">
         <v>2538</v>
       </c>
-      <c r="P9" s="24">
+      <c r="P9">
         <v>2997</v>
       </c>
       <c r="Q9"/>
@@ -1738,16 +1760,16 @@
       <c r="K10" s="18">
         <v>2185</v>
       </c>
-      <c r="M10" s="23" t="s">
+      <c r="M10" s="22" t="s">
         <v>33</v>
       </c>
-      <c r="N10" s="24">
+      <c r="N10">
         <v>4461</v>
       </c>
-      <c r="O10" s="24">
+      <c r="O10">
         <v>3078</v>
       </c>
-      <c r="P10" s="24">
+      <c r="P10">
         <v>3769.5</v>
       </c>
       <c r="Q10"/>
@@ -1804,12 +1826,12 @@
       <c r="K11" s="18">
         <v>3547</v>
       </c>
-      <c r="M11" s="23" t="s">
+      <c r="M11" s="22" t="s">
         <v>35</v>
       </c>
-      <c r="N11" s="24"/>
-      <c r="O11" s="24"/>
-      <c r="P11" s="24"/>
+      <c r="N11"/>
+      <c r="O11"/>
+      <c r="P11"/>
       <c r="Q11"/>
       <c r="R11"/>
       <c r="S11"/>
@@ -1862,16 +1884,16 @@
       <c r="K12" s="18">
         <v>1681</v>
       </c>
-      <c r="M12" s="23" t="s">
+      <c r="M12" s="22" t="s">
         <v>37</v>
       </c>
-      <c r="N12" s="24">
+      <c r="N12">
         <v>4879</v>
       </c>
-      <c r="O12" s="24">
+      <c r="O12">
         <v>3453</v>
       </c>
-      <c r="P12" s="24">
+      <c r="P12">
         <v>4166</v>
       </c>
       <c r="Q12"/>
@@ -1928,16 +1950,16 @@
       <c r="K13" s="14">
         <v>2552</v>
       </c>
-      <c r="M13" s="23" t="s">
+      <c r="M13" s="22" t="s">
         <v>39</v>
       </c>
-      <c r="N13" s="24">
+      <c r="N13">
         <v>3340</v>
       </c>
-      <c r="O13" s="24">
+      <c r="O13">
         <v>2459</v>
       </c>
-      <c r="P13" s="24">
+      <c r="P13">
         <v>2899.5</v>
       </c>
       <c r="Q13"/>
@@ -1992,12 +2014,12 @@
       <c r="K14" s="14">
         <v>2223</v>
       </c>
-      <c r="M14" s="22" t="s">
+      <c r="M14" s="21" t="s">
         <v>11</v>
       </c>
-      <c r="N14" s="24"/>
-      <c r="O14" s="24"/>
-      <c r="P14" s="24"/>
+      <c r="N14"/>
+      <c r="O14"/>
+      <c r="P14"/>
       <c r="Q14"/>
       <c r="R14"/>
       <c r="S14"/>
@@ -2052,16 +2074,16 @@
       <c r="K15" s="14">
         <v>3641</v>
       </c>
-      <c r="M15" s="23" t="s">
+      <c r="M15" s="22" t="s">
         <v>25</v>
       </c>
-      <c r="N15" s="24">
+      <c r="N15">
         <v>2506</v>
       </c>
-      <c r="O15" s="24">
+      <c r="O15">
         <v>1756</v>
       </c>
-      <c r="P15" s="24">
+      <c r="P15">
         <v>2131</v>
       </c>
       <c r="Q15"/>
@@ -2116,16 +2138,16 @@
       <c r="K16" s="14">
         <v>1734</v>
       </c>
-      <c r="M16" s="23" t="s">
+      <c r="M16" s="22" t="s">
         <v>27</v>
       </c>
-      <c r="N16" s="24">
+      <c r="N16">
         <v>2177</v>
       </c>
-      <c r="O16" s="24">
+      <c r="O16">
         <v>1599</v>
       </c>
-      <c r="P16" s="24">
+      <c r="P16">
         <v>1888</v>
       </c>
       <c r="Q16"/>
@@ -2182,16 +2204,16 @@
       <c r="K17" s="14">
         <v>2626</v>
       </c>
-      <c r="M17" s="23" t="s">
+      <c r="M17" s="22" t="s">
         <v>29</v>
       </c>
-      <c r="N17" s="24">
+      <c r="N17">
         <v>2434</v>
       </c>
-      <c r="O17" s="24">
+      <c r="O17">
         <v>1938</v>
       </c>
-      <c r="P17" s="24">
+      <c r="P17">
         <v>2186</v>
       </c>
       <c r="Q17"/>
@@ -2246,16 +2268,16 @@
       <c r="K18" s="14">
         <v>2248</v>
       </c>
-      <c r="M18" s="23" t="s">
+      <c r="M18" s="22" t="s">
         <v>31</v>
       </c>
-      <c r="N18" s="24">
+      <c r="N18">
         <v>2252</v>
       </c>
-      <c r="O18" s="24">
+      <c r="O18">
         <v>1834</v>
       </c>
-      <c r="P18" s="24">
+      <c r="P18">
         <v>2043</v>
       </c>
       <c r="Q18"/>
@@ -2312,12 +2334,12 @@
       <c r="K19" s="14">
         <v>3724</v>
       </c>
-      <c r="M19" s="23" t="s">
+      <c r="M19" s="22" t="s">
         <v>33</v>
       </c>
-      <c r="N19" s="24"/>
-      <c r="O19" s="24"/>
-      <c r="P19" s="24"/>
+      <c r="N19"/>
+      <c r="O19"/>
+      <c r="P19"/>
       <c r="Q19"/>
       <c r="R19"/>
       <c r="S19"/>
@@ -2370,16 +2392,16 @@
       <c r="K20" s="14">
         <v>1750</v>
       </c>
-      <c r="M20" s="23" t="s">
+      <c r="M20" s="22" t="s">
         <v>35</v>
       </c>
-      <c r="N20" s="24">
+      <c r="N20">
         <v>2418</v>
       </c>
-      <c r="O20" s="24">
+      <c r="O20">
         <v>1918</v>
       </c>
-      <c r="P20" s="24">
+      <c r="P20">
         <v>2168</v>
       </c>
       <c r="Q20"/>
@@ -2436,12 +2458,12 @@
       <c r="K21" s="14">
         <v>2680</v>
       </c>
-      <c r="M21" s="23" t="s">
+      <c r="M21" s="22" t="s">
         <v>37</v>
       </c>
-      <c r="N21" s="24"/>
-      <c r="O21" s="24"/>
-      <c r="P21" s="24"/>
+      <c r="N21"/>
+      <c r="O21"/>
+      <c r="P21"/>
       <c r="Q21"/>
       <c r="R21"/>
       <c r="S21"/>
@@ -2465,44 +2487,44 @@
       <c r="AK21"/>
     </row>
     <row r="22" spans="1:37" x14ac:dyDescent="0.25">
-      <c r="M22" s="23" t="s">
+      <c r="M22" s="22" t="s">
         <v>39</v>
       </c>
-      <c r="N22" s="24">
+      <c r="N22">
         <v>2103</v>
       </c>
-      <c r="O22" s="24">
+      <c r="O22">
         <v>1616</v>
       </c>
-      <c r="P22" s="24">
+      <c r="P22">
         <v>1859.5</v>
       </c>
     </row>
     <row r="23" spans="1:37" x14ac:dyDescent="0.25">
-      <c r="M23" s="22" t="s">
+      <c r="M23" s="21" t="s">
         <v>26</v>
       </c>
-      <c r="N23" s="24">
+      <c r="N23">
         <v>2820.5</v>
       </c>
-      <c r="O23" s="24">
+      <c r="O23">
         <v>1974.5</v>
       </c>
-      <c r="P23" s="24">
+      <c r="P23">
         <v>2397.5</v>
       </c>
     </row>
     <row r="24" spans="1:37" x14ac:dyDescent="0.25">
-      <c r="M24" s="22" t="s">
+      <c r="M24" s="21" t="s">
         <v>28</v>
       </c>
-      <c r="N24" s="24">
+      <c r="N24">
         <v>2416</v>
       </c>
-      <c r="O24" s="24">
+      <c r="O24">
         <v>1886</v>
       </c>
-      <c r="P24" s="24">
+      <c r="P24">
         <v>2151</v>
       </c>
     </row>
@@ -2532,16 +2554,16 @@
       <c r="K25" s="15">
         <v>270967</v>
       </c>
-      <c r="M25" s="22" t="s">
+      <c r="M25" s="21" t="s">
         <v>30</v>
       </c>
-      <c r="N25" s="24">
+      <c r="N25">
         <v>2966.5</v>
       </c>
-      <c r="O25" s="24">
+      <c r="O25">
         <v>2277.5</v>
       </c>
-      <c r="P25" s="24">
+      <c r="P25">
         <v>2622</v>
       </c>
     </row>
@@ -2575,44 +2597,44 @@
       <c r="K26" s="11">
         <v>489224</v>
       </c>
-      <c r="M26" s="22" t="s">
+      <c r="M26" s="21" t="s">
         <v>32</v>
       </c>
-      <c r="N26" s="24">
+      <c r="N26">
         <v>2854</v>
       </c>
-      <c r="O26" s="24">
+      <c r="O26">
         <v>2186</v>
       </c>
-      <c r="P26" s="24">
+      <c r="P26">
         <v>2520</v>
       </c>
     </row>
     <row r="27" spans="1:37" x14ac:dyDescent="0.25">
-      <c r="M27" s="22" t="s">
+      <c r="M27" s="21" t="s">
         <v>34</v>
       </c>
-      <c r="N27" s="24">
+      <c r="N27">
         <v>4461</v>
       </c>
-      <c r="O27" s="24">
+      <c r="O27">
         <v>3078</v>
       </c>
-      <c r="P27" s="24">
+      <c r="P27">
         <v>3769.5</v>
       </c>
     </row>
     <row r="28" spans="1:37" x14ac:dyDescent="0.25">
-      <c r="M28" s="22" t="s">
+      <c r="M28" s="21" t="s">
         <v>36</v>
       </c>
-      <c r="N28" s="24">
+      <c r="N28">
         <v>2418</v>
       </c>
-      <c r="O28" s="24">
+      <c r="O28">
         <v>1918</v>
       </c>
-      <c r="P28" s="24">
+      <c r="P28">
         <v>2168</v>
       </c>
     </row>
@@ -2642,16 +2664,16 @@
       <c r="K29" s="15">
         <v>43495</v>
       </c>
-      <c r="M29" s="22" t="s">
+      <c r="M29" s="21" t="s">
         <v>38</v>
       </c>
-      <c r="N29" s="24">
+      <c r="N29">
         <v>4879</v>
       </c>
-      <c r="O29" s="24">
+      <c r="O29">
         <v>3453</v>
       </c>
-      <c r="P29" s="24">
+      <c r="P29">
         <v>4166</v>
       </c>
     </row>
@@ -2682,16 +2704,16 @@
       <c r="K30" s="15">
         <v>95346</v>
       </c>
-      <c r="M30" s="22" t="s">
+      <c r="M30" s="21" t="s">
         <v>40</v>
       </c>
-      <c r="N30" s="24">
+      <c r="N30">
         <v>2721.5</v>
       </c>
-      <c r="O30" s="24">
+      <c r="O30">
         <v>2037.5</v>
       </c>
-      <c r="P30" s="24">
+      <c r="P30">
         <v>2379.5</v>
       </c>
     </row>

</xml_diff>